<commit_message>
complete individual components of table
</commit_message>
<xml_diff>
--- a/tables.xlsx
+++ b/tables.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="19">
   <si>
     <t>label</t>
   </si>
@@ -64,6 +64,18 @@
   </si>
   <si>
     <t>Sports</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>precision</t>
+  </si>
+  <si>
+    <t>recall</t>
+  </si>
+  <si>
+    <t>F Measure</t>
   </si>
 </sst>
 </file>
@@ -120,8 +132,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -149,7 +165,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="27">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -161,6 +177,8 @@
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -172,6 +190,8 @@
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -501,10 +521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -515,7 +535,7 @@
     <col min="4" max="4" width="20.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -540,8 +560,17 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="I1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -567,8 +596,17 @@
       <c r="H2">
         <v>43</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="I2">
+        <v>0.5</v>
+      </c>
+      <c r="J2">
+        <v>2.2727270000000001E-2</v>
+      </c>
+      <c r="K2">
+        <v>4.3478259999999998E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -594,8 +632,17 @@
       <c r="H3">
         <v>106</v>
       </c>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="I3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -621,8 +668,17 @@
       <c r="H4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="I4">
+        <v>0.76749999999999996</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -648,8 +704,17 @@
       <c r="H5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="I5">
+        <v>0.625</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>0.86845826999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -675,8 +740,17 @@
       <c r="H6">
         <v>286</v>
       </c>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="I6" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0.76923076999999995</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -702,8 +776,17 @@
       <c r="H7">
         <v>149</v>
       </c>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="I7" t="s">
+        <v>15</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -729,8 +812,22 @@
       <c r="H8">
         <v>28</v>
       </c>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="I8" t="s">
+        <v>15</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="K9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
@@ -755,8 +852,17 @@
       <c r="H11" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="12" spans="1:8">
+      <c r="I11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -767,7 +873,7 @@
         <v>0.11083333333333301</v>
       </c>
       <c r="D12">
-        <v>0.56388158775570496</v>
+        <v>0.60087484409242498</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -781,8 +887,17 @@
       <c r="H12">
         <v>266</v>
       </c>
-    </row>
-    <row r="13" spans="1:8">
+      <c r="I12" t="s">
+        <v>15</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -793,22 +908,31 @@
         <v>0.26333333333333298</v>
       </c>
       <c r="D13">
-        <v>0.61076185786500903</v>
+        <v>0.60348423151275399</v>
       </c>
       <c r="E13">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F13">
-        <v>1751</v>
+        <v>1755</v>
       </c>
       <c r="G13">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="H13">
-        <v>620</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
+        <v>624</v>
+      </c>
+      <c r="I13">
+        <v>0.61904761904761896</v>
+      </c>
+      <c r="J13">
+        <v>2.04081632653061E-2</v>
+      </c>
+      <c r="K13">
+        <v>3.9513677811550199E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -819,7 +943,7 @@
         <v>0.288333333333333</v>
       </c>
       <c r="D14">
-        <v>0.56560888237603402</v>
+        <v>0.55947191726117096</v>
       </c>
       <c r="E14">
         <v>1708</v>
@@ -833,86 +957,122 @@
       <c r="H14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:8">
+      <c r="I14">
+        <v>0.711666666666667</v>
+      </c>
+      <c r="J14">
+        <v>1</v>
+      </c>
+      <c r="K14">
+        <v>0.83154819863680596</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
       <c r="A15" t="s">
         <v>11</v>
       </c>
       <c r="B15">
-        <v>0.64291666666666702</v>
+        <v>0.64041666666666697</v>
       </c>
       <c r="C15">
-        <v>0.35708333333333298</v>
+        <v>0.35958333333333298</v>
       </c>
       <c r="D15">
-        <v>0.49503882137345701</v>
+        <v>0.522219057436343</v>
       </c>
       <c r="E15">
         <v>1536</v>
       </c>
       <c r="F15">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="G15">
-        <v>857</v>
+        <v>863</v>
       </c>
       <c r="H15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:8">
+      <c r="I15">
+        <v>0.64026677782409303</v>
+      </c>
+      <c r="J15">
+        <v>1</v>
+      </c>
+      <c r="K15">
+        <v>0.78068614993646801</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
       <c r="A16" t="s">
         <v>12</v>
       </c>
       <c r="B16">
-        <v>0.75583333333333302</v>
+        <v>0.757083333333333</v>
       </c>
       <c r="C16">
-        <v>0.244166666666667</v>
+        <v>0.242916666666667</v>
       </c>
       <c r="D16">
-        <v>0.518530441013073</v>
+        <v>0.50427117248853304</v>
       </c>
       <c r="E16">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F16">
-        <v>1810</v>
+        <v>1817</v>
       </c>
       <c r="G16">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="H16">
-        <v>579</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
+        <v>583</v>
+      </c>
+      <c r="I16" t="s">
+        <v>15</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
       <c r="A17" t="s">
         <v>13</v>
       </c>
       <c r="B17">
-        <v>0.65083333333333304</v>
+        <v>0.64958333333333296</v>
       </c>
       <c r="C17">
-        <v>0.34916666666666701</v>
+        <v>0.35041666666666699</v>
       </c>
       <c r="D17">
-        <v>0.54994505494505497</v>
+        <v>0.54569024725274795</v>
       </c>
       <c r="E17">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F17">
-        <v>1559</v>
+        <v>1553</v>
       </c>
       <c r="G17">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="H17">
-        <v>837</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
+        <v>834</v>
+      </c>
+      <c r="I17">
+        <v>0.46153846153846201</v>
+      </c>
+      <c r="J17">
+        <v>7.14285714285714E-3</v>
+      </c>
+      <c r="K17">
+        <v>1.4067995310668199E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -923,7 +1083,7 @@
         <v>8.7083333333333304E-2</v>
       </c>
       <c r="D18">
-        <v>0.58545943714936599</v>
+        <v>0.55548688741895402</v>
       </c>
       <c r="E18">
         <v>0</v>
@@ -936,6 +1096,15 @@
       </c>
       <c r="H18">
         <v>209</v>
+      </c>
+      <c r="I18" t="s">
+        <v>15</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>